<commit_message>
completed login module for other modules
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DsPortalTestData.xlsx
+++ b/src/test/resources/TestData/DsPortalTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devaki Girirajan\eclipse-workspace\DsAlgoTestNG2025\TestNG\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devaki Girirajan\eclipse-workspace\DsAlgoTestNG2025\TestNG\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CB2EC3-D4FD-4A9F-929C-890522F60DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F1070B-8D1A-41ED-B78E-B213165F610B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{5E5F66B2-BA7B-446B-98B9-F591A5400595}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5E5F66B2-BA7B-446B-98B9-F591A5400595}"/>
   </bookViews>
   <sheets>
     <sheet name="LogIn" sheetId="1" r:id="rId1"/>
@@ -158,11 +158,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -503,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCD9D7F-0F4D-477B-9ABF-A17956C1B1A0}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,35 +513,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -559,57 +557,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13239840-227E-470D-AE41-1D60312EB11B}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>